<commit_message>
melhoria nos relatórios para economizar papel
mudança no template da planilha, para mostrar o valor dos produtos
somente 1 vez, e não a cada página. remoção do contato do cestante do
relatório de pedidos que é utilizado pelo responsável pela entrega.
criação de um relatório específico com todas as informações de contato
dos cestantes que fizeram pedido na respectiva chamada.
</commit_message>
<xml_diff>
--- a/arquivos/modelo_relatorio_pedidos_para_nucleo.xlsx
+++ b/arquivos/modelo_relatorio_pedidos_para_nucleo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="21840" windowHeight="9000"/>
+    <workbookView xWindow="0" yWindow="48" windowWidth="21840" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="modelo" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">modelo!$A:$D</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">modelo!$A:$B</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -362,75 +362,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" style="1" customWidth="1"/>
-    <col min="3" max="4" width="8.85546875" style="1" customWidth="1"/>
-    <col min="5" max="34" width="6.7109375" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="29.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="8.88671875" style="1" customWidth="1"/>
+    <col min="5" max="34" width="6.6640625" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
melhoria no arquivo modelo do relatorio
melhoria no arquivo modelo do relatorio de pedidos para os nucleos
</commit_message>
<xml_diff>
--- a/arquivos/modelo_relatorio_pedidos_para_nucleo.xlsx
+++ b/arquivos/modelo_relatorio_pedidos_para_nucleo.xlsx
@@ -4,13 +4,35 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="48" windowWidth="21840" windowHeight="9000"/>
+    <workbookView xWindow="0" yWindow="48" windowWidth="15576" windowHeight="9000"/>
   </bookViews>
   <sheets>
-    <sheet name="modelo" sheetId="1" r:id="rId1"/>
+    <sheet name="nucleo1" sheetId="11" r:id="rId1"/>
+    <sheet name="nucleo2" sheetId="10" r:id="rId2"/>
+    <sheet name="nucleo3" sheetId="9" r:id="rId3"/>
+    <sheet name="nucleo4" sheetId="8" r:id="rId4"/>
+    <sheet name="nucleo5" sheetId="7" r:id="rId5"/>
+    <sheet name="nucleo6" sheetId="6" r:id="rId6"/>
+    <sheet name="nucleo7" sheetId="5" r:id="rId7"/>
+    <sheet name="nucleo8" sheetId="4" r:id="rId8"/>
+    <sheet name="nucleo9" sheetId="3" r:id="rId9"/>
+    <sheet name="nucleo10" sheetId="2" r:id="rId10"/>
+    <sheet name="nucleo11" sheetId="1" r:id="rId11"/>
+    <sheet name="nucleo12" sheetId="12" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">modelo!$A:$B</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">nucleo1!$A:$B</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="9">nucleo10!$A:$B</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="10">nucleo11!$A:$B</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="11">nucleo12!$A:$B</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">nucleo2!$A:$B</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">nucleo3!$A:$B</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">nucleo4!$A:$B</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="4">nucleo5!$A:$B</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="5">nucleo6!$A:$B</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="6">nucleo7!$A:$B</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="7">nucleo8!$A:$B</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="8">nucleo9!$A:$B</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -74,9 +96,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -114,7 +136,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -186,7 +208,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -362,7 +384,834 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="8.88671875" style="1" customWidth="1"/>
+    <col min="5" max="34" width="6.6640625" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A109"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="8.88671875" style="1" customWidth="1"/>
+    <col min="5" max="34" width="6.6640625" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A109"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="8.88671875" style="1" customWidth="1"/>
+    <col min="5" max="34" width="6.6640625" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A109"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="8.88671875" style="1" customWidth="1"/>
+    <col min="5" max="34" width="6.6640625" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A109"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="8.88671875" style="1" customWidth="1"/>
+    <col min="5" max="34" width="6.6640625" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A109"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="8.88671875" style="1" customWidth="1"/>
+    <col min="5" max="34" width="6.6640625" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A109"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="8.88671875" style="1" customWidth="1"/>
+    <col min="5" max="34" width="6.6640625" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A109"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="8.88671875" style="1" customWidth="1"/>
+    <col min="5" max="34" width="6.6640625" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A109"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="8.88671875" style="1" customWidth="1"/>
+    <col min="5" max="34" width="6.6640625" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A109"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="8.88671875" style="1" customWidth="1"/>
+    <col min="5" max="34" width="6.6640625" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A109"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="8.88671875" style="1" customWidth="1"/>
+    <col min="5" max="34" width="6.6640625" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A109"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>